<commit_message>
10 band filter calc + sim 3rd order
</commit_message>
<xml_diff>
--- a/Simulation/Calculations/Filters/FiltersCalc.xlsx
+++ b/Simulation/Calculations/Filters/FiltersCalc.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Repo\Git\rftools\Simulation\Calculations\Filters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikguz/Documents/git/github/rftools/Simulation/Calculations/Filters/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50360" windowHeight="25960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chebyshev LPF" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,12 @@
     <sheet name="Bessel LPF" sheetId="3" r:id="rId4"/>
     <sheet name="NormalizedValues" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Cutoff frequency (Hz)</t>
   </si>
@@ -100,15 +103,33 @@
   </si>
   <si>
     <t xml:space="preserve">C3 </t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>20m</t>
+  </si>
+  <si>
+    <t>Results - 6m</t>
+  </si>
+  <si>
+    <t>Results - 10m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -147,18 +168,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,7 +495,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -488,22 +509,22 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
-    <col min="19" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="19" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>54000000</v>
       </c>
@@ -633,7 +654,7 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K3">
         <f t="shared" ref="K3:K8" si="0">(V3)/(2*PI()*$A$2*$F$2)</f>
         <v>5.8946275219220494E-11</v>
@@ -664,7 +685,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K4">
         <f t="shared" si="0"/>
         <v>4.509390054270368E-11</v>
@@ -697,7 +718,7 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K5">
         <f t="shared" si="0"/>
         <v>8.3350033159977779E-11</v>
@@ -732,7 +753,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K6">
         <f t="shared" si="0"/>
         <v>8.3350033159977779E-11</v>
@@ -769,7 +790,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K7">
         <f t="shared" si="0"/>
         <v>8.3350033159977779E-11</v>
@@ -808,7 +829,7 @@
       </c>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K8">
         <f t="shared" si="0"/>
         <v>8.3350033159977779E-11</v>
@@ -857,303 +878,363 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" customWidth="1"/>
-    <col min="26" max="26" width="12" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="27" max="27" width="13.5" customWidth="1"/>
+    <col min="28" max="28" width="12" customWidth="1"/>
+    <col min="29" max="29" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
         <v>54000000</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>108000000</v>
-      </c>
       <c r="D2">
+        <v>60000000</v>
+      </c>
+      <c r="E2">
         <v>3</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="I2">
         <v>52000000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4000000</v>
       </c>
-      <c r="K2">
-        <f>(Y2)/(2*PI()*$I$2*$F$2)</f>
+      <c r="M2">
+        <f>(AA2)/(2*PI()*$J$2*$G$2)</f>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="L2" s="3">
-        <f>($F$2*$I$2)/(2*PI()*POWER($H$2,2)*Y2)</f>
+      <c r="N2" s="3">
+        <f>($G$2*$J$2)/(2*PI()*POWER($I$2,2)*AA2)</f>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="M2">
-        <f>(Z2*$F$2)/(2*PI()*$I$2)</f>
+      <c r="O2">
+        <f>(AB2*$G$2)/(2*PI()*$J$2)</f>
         <v>2.8130636191492502E-6</v>
       </c>
-      <c r="N2" s="3">
-        <f>($I$2)/(2*PI()*POWER($H$2,2)*$F$2*Z2)</f>
+      <c r="P2" s="3">
+        <f>($J$2)/(2*PI()*POWER($I$2,2)*$G$2*AB2)</f>
         <v>3.330075054440702E-12</v>
       </c>
-      <c r="O2">
-        <f>(AA2)/(2*PI()*$I$2*$F$2)</f>
+      <c r="Q2">
+        <f>(AC2)/(2*PI()*$J$2*$G$2)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="4" t="e">
-        <f>($F$2*$I$2)/(2*PI()*POWER($H$2,2)*AA2)</f>
+      <c r="R2" s="4" t="e">
+        <f>($G$2*$J$2)/(2*PI()*POWER($I$2,2)*AC2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>2</v>
       </c>
-      <c r="Y2" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
+      <c r="AA2" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1.4139999999999999</v>
+      </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="0">(Y3)/(2*PI()*$I$2*$F$2)</f>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>29700000</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>40000000</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>28850000</v>
+      </c>
+      <c r="J3">
+        <v>3000000</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="0">(AA3)/(2*PI()*$J$2*$G$2)</f>
         <v>7.9577471545947675E-10</v>
       </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L8" si="1">($F$2*$I$2)/(2*PI()*POWER($H$2,2)*Y3)</f>
+      <c r="N3" s="3">
+        <f t="shared" ref="N3:N8" si="1">($G$2*$J$2)/(2*PI()*POWER($I$2,2)*AA3)</f>
         <v>1.177181531744788E-8</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M8" si="2">(Z3*$F$2)/(2*PI()*$I$2)</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="2">(AB3*$G$2)/(2*PI()*$J$2)</f>
         <v>3.9788735772973834E-6</v>
       </c>
-      <c r="N3" s="3">
-        <f>($I$2)/(2*PI()*POWER($H$2,2)*$F$2*Z3)</f>
+      <c r="P3" s="3">
+        <f>($J$2)/(2*PI()*POWER($I$2,2)*$G$2*AB3)</f>
         <v>2.354363063489576E-12</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O8" si="3">(AA3)/(2*PI()*$I$2*$F$2)</f>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q8" si="3">(AC3)/(2*PI()*$J$2*$G$2)</f>
         <v>7.9577471545947675E-10</v>
       </c>
-      <c r="P3" s="4">
-        <f t="shared" ref="P3:P8" si="4">($F$2*$I$2)/(2*PI()*POWER($H$2,2)*AA3)</f>
+      <c r="R3" s="4">
+        <f t="shared" ref="R3:R8" si="4">($G$2*$J$2)/(2*PI()*POWER($I$2,2)*AC3)</f>
         <v>1.177181531744788E-8</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>3</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>2</v>
       </c>
       <c r="AA3" s="1">
         <v>1</v>
       </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
+      <c r="AB3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K4">
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>14350000</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>16000000</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>14175000</v>
+      </c>
+      <c r="J4">
+        <v>350000</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="0"/>
         <v>6.0876765732649971E-10</v>
       </c>
-      <c r="L4" s="3">
+      <c r="N4" s="3">
         <f t="shared" si="1"/>
         <v>1.5387993879016835E-8</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <f t="shared" si="2"/>
         <v>3.6764791854227826E-6</v>
       </c>
-      <c r="N4" s="3">
-        <f t="shared" ref="N3:N8" si="5">($I$2)/(2*PI()*POWER($H$2,2)*$F$2*Z4)</f>
+      <c r="P4" s="3">
+        <f t="shared" ref="P4:P8" si="5">($J$2)/(2*PI()*POWER($I$2,2)*$G$2*AB4)</f>
         <v>2.5480119734735671E-12</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <f t="shared" si="3"/>
         <v>1.4705916741691131E-9</v>
       </c>
-      <c r="P4" s="4">
+      <c r="R4" s="4">
         <f t="shared" si="4"/>
         <v>6.3700299336839176E-9</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>4</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="AA4" s="2">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AB4" s="2">
         <v>1.8480000000000001</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AC4" s="2">
         <v>1.8480000000000001</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AD4" s="2">
         <v>0.76500000000000001</v>
       </c>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K5">
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M5">
         <f t="shared" si="0"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="L5" s="3">
+      <c r="N5" s="3">
         <f t="shared" si="1"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <f t="shared" si="2"/>
         <v>2.8130636191492502E-6</v>
       </c>
-      <c r="N5" s="3">
+      <c r="P5" s="3">
         <f t="shared" si="5"/>
         <v>3.330075054440702E-12</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <f t="shared" si="3"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="P5" s="4">
+      <c r="R5" s="4">
         <f t="shared" si="4"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>5</v>
       </c>
-      <c r="Y5" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1.4139999999999999</v>
-      </c>
       <c r="AA5" s="1">
         <v>1.4139999999999999</v>
       </c>
@@ -1163,44 +1244,44 @@
       <c r="AC5" s="1">
         <v>1.4139999999999999</v>
       </c>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
+      <c r="AD5" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>1.4139999999999999</v>
+      </c>
       <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K6">
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="L6" s="3">
+      <c r="N6" s="3">
         <f t="shared" si="1"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <f t="shared" si="2"/>
         <v>2.8130636191492502E-6</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <f t="shared" si="5"/>
         <v>3.330075054440702E-12</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <f t="shared" si="3"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="P6" s="4">
+      <c r="R6" s="4">
         <f t="shared" si="4"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>6</v>
       </c>
-      <c r="Y6" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1.4139999999999999</v>
-      </c>
       <c r="AA6" s="1">
         <v>1.4139999999999999</v>
       </c>
@@ -1213,43 +1294,43 @@
       <c r="AD6" s="1">
         <v>1.4139999999999999</v>
       </c>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K7">
+      <c r="AE6" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="L7" s="3">
+      <c r="N7" s="3">
         <f t="shared" si="1"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <f t="shared" si="2"/>
         <v>2.8130636191492502E-6</v>
       </c>
-      <c r="N7" s="3">
+      <c r="P7" s="3">
         <f t="shared" si="5"/>
         <v>3.330075054440702E-12</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <f t="shared" si="3"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="P7" s="4">
+      <c r="R7" s="4">
         <f t="shared" si="4"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>7</v>
       </c>
-      <c r="Y7" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1.4139999999999999</v>
-      </c>
       <c r="AA7" s="1">
         <v>1.4139999999999999</v>
       </c>
@@ -1265,42 +1346,42 @@
       <c r="AE7" s="1">
         <v>1.4139999999999999</v>
       </c>
-      <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K8">
+      <c r="AF7" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="L8" s="3">
+      <c r="N8" s="3">
         <f t="shared" si="1"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <f t="shared" si="2"/>
         <v>2.8130636191492502E-6</v>
       </c>
-      <c r="N8" s="3">
+      <c r="P8" s="3">
         <f t="shared" si="5"/>
         <v>3.330075054440702E-12</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <f t="shared" si="3"/>
         <v>1.1252254476597001E-9</v>
       </c>
-      <c r="P8" s="4">
+      <c r="R8" s="4">
         <f t="shared" si="4"/>
         <v>8.3251876361017539E-9</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>8</v>
       </c>
-      <c r="Y8" s="1">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>1.4139999999999999</v>
-      </c>
       <c r="AA8" s="1">
         <v>1.4139999999999999</v>
       </c>
@@ -1319,6 +1400,242 @@
       <c r="AF8" s="1">
         <v>1.4139999999999999</v>
       </c>
+      <c r="AG8" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>18</v>
+      </c>
+      <c r="S10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" t="s">
+        <v>7</v>
+      </c>
+      <c r="U10" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10" t="s">
+        <v>9</v>
+      </c>
+      <c r="W10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <f>(AA2)/(2*PI()*$J$3*$G$3)</f>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="N11" s="3">
+        <f>($G$3*$J$3)/(2*PI()*POWER($I$3,2)*AA2)</f>
+        <v>2.0284782071870407E-8</v>
+      </c>
+      <c r="O11">
+        <f>(AB2*$G$3)/(2*PI()*$J$3)</f>
+        <v>3.7507514921990002E-6</v>
+      </c>
+      <c r="P11" s="3">
+        <f>($J$3)/(2*PI()*POWER($I$3,2)*$G$3*AB2)</f>
+        <v>8.1139128287481631E-12</v>
+      </c>
+      <c r="Q11">
+        <f>(AC2)/(2*PI()*$J$3*$G$3)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4" t="e">
+        <f>($G$3*$J$3)/(2*PI()*POWER($I$3,2)*AC2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <f>(AA3)/(2*PI()*$J$3*$G$3)</f>
+        <v>1.0610329539459691E-9</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" ref="N12:N19" si="6">($G$3*$J$3)/(2*PI()*POWER($I$3,2)*AA3)</f>
+        <v>2.8682681849624756E-8</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O19" si="7">(AB3*$G$3)/(2*PI()*$J$3)</f>
+        <v>5.3051647697298443E-6</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" ref="P12:P19" si="8">($J$3)/(2*PI()*POWER($I$3,2)*$G$3*AB3)</f>
+        <v>5.7365363699249513E-12</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12:Q19" si="9">(AC3)/(2*PI()*$J$3*$G$3)</f>
+        <v>1.0610329539459691E-9</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" ref="R12:R19" si="10">($G$3*$J$3)/(2*PI()*POWER($I$3,2)*AC3)</f>
+        <v>2.8682681849624756E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <f t="shared" ref="M12:M19" si="11">(AA4)/(2*PI()*$J$3*$G$3)</f>
+        <v>8.1169020976866625E-10</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="6"/>
+        <v>3.7493701764215372E-8</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="7"/>
+        <v>4.9019722472303765E-6</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" si="8"/>
+        <v>6.2083726947239735E-12</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="9"/>
+        <v>1.9607888988921507E-9</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="10"/>
+        <v>1.5520931736809931E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <f t="shared" si="11"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="6"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="7"/>
+        <v>3.7507514921990002E-6</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="8"/>
+        <v>8.1139128287481631E-12</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="9"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="10"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <f t="shared" si="11"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="6"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="7"/>
+        <v>3.7507514921990002E-6</v>
+      </c>
+      <c r="P15" s="3">
+        <f t="shared" si="8"/>
+        <v>8.1139128287481631E-12</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="9"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="10"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <f t="shared" si="11"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="6"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="7"/>
+        <v>3.7507514921990002E-6</v>
+      </c>
+      <c r="P16" s="3">
+        <f t="shared" si="8"/>
+        <v>8.1139128287481631E-12</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="9"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="10"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="13:18" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <f t="shared" si="11"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="6"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="7"/>
+        <v>3.7507514921990002E-6</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" si="8"/>
+        <v>8.1139128287481631E-12</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="9"/>
+        <v>1.5003005968796E-9</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="10"/>
+        <v>2.0284782071870407E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="13:18" x14ac:dyDescent="0.2">
+      <c r="N18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="13:18" x14ac:dyDescent="0.2">
+      <c r="N19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="R19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1331,7 +1648,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1343,7 +1660,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>